<commit_message>
updated Honduras sites and added Philippines data migration
</commit_message>
<xml_diff>
--- a/data/preprocessed/honduras/ff2.0/hon_ff2.0_fish_sites_preprocessed.xlsx
+++ b/data/preprocessed/honduras/ff2.0/hon_ff2.0_fish_sites_preprocessed.xlsx
@@ -600,6 +600,12 @@
           <t>glca1</t>
         </is>
       </c>
+      <c r="C7">
+        <v>16.4606</v>
+      </c>
+      <c r="D7">
+        <v>-85.82510000000001</v>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -617,6 +623,12 @@
           <t>glca2</t>
         </is>
       </c>
+      <c r="C8">
+        <v>16.44315</v>
+      </c>
+      <c r="D8">
+        <v>-85.8612</v>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -634,6 +646,12 @@
           <t>glca4</t>
         </is>
       </c>
+      <c r="C9">
+        <v>16.4504</v>
+      </c>
+      <c r="D9">
+        <v>-85.8623</v>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -651,6 +669,12 @@
           <t>glia1</t>
         </is>
       </c>
+      <c r="C10">
+        <v>16.4199</v>
+      </c>
+      <c r="D10">
+        <v>-85.90000000000001</v>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -668,6 +692,12 @@
           <t>gmc3</t>
         </is>
       </c>
+      <c r="C11">
+        <v>16.5555</v>
+      </c>
+      <c r="D11">
+        <v>-85.89919999999999</v>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -685,6 +715,12 @@
           <t>gmca2</t>
         </is>
       </c>
+      <c r="C12">
+        <v>16.4702</v>
+      </c>
+      <c r="D12">
+        <v>-85.90260000000001</v>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -1036,6 +1072,12 @@
           <t>bajo_costa_azul_1</t>
         </is>
       </c>
+      <c r="C24">
+        <v>15.909713</v>
+      </c>
+      <c r="D24">
+        <v>-87.930267</v>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -1053,6 +1095,12 @@
           <t>bajo_costa_azul_2</t>
         </is>
       </c>
+      <c r="C25">
+        <v>15.887213</v>
+      </c>
+      <c r="D25">
+        <v>-87.936851</v>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -1087,6 +1135,12 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C27">
+        <v>16.393</v>
+      </c>
+      <c r="D27">
+        <v>-86.274</v>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -1206,6 +1260,12 @@
           <t>6</t>
         </is>
       </c>
+      <c r="C34">
+        <v>16.374</v>
+      </c>
+      <c r="D34">
+        <v>-86.283</v>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>Honduras</t>
@@ -1222,6 +1282,12 @@
         <is>
           <t>7</t>
         </is>
+      </c>
+      <c r="C35">
+        <v>16.358</v>
+      </c>
+      <c r="D35">
+        <v>-86.289</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>

</xml_diff>